<commit_message>
Updated the first table to use NPC1 instead of CAR2.
</commit_message>
<xml_diff>
--- a/functional_scenarios/atomic_blocks.xlsx
+++ b/functional_scenarios/atomic_blocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Embry Riddle\One Drive\Embry-Riddle Aeronautical University\Akbas Research - Documents\General\Projects\Foretellix\Accidents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\xlsx2tex\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D755813B-1C66-4991-8B32-C18DB1D67D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0228EC4C-86B6-445F-B18E-59B061DBA5BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="-14190" windowWidth="21600" windowHeight="11385" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(1S) Edges" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="(3MP) 5-way Intersection-w-Pd" sheetId="14" r:id="rId13"/>
     <sheet name="Key" sheetId="3" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="276">
   <si>
     <t>ID</t>
   </si>
@@ -874,13 +874,25 @@
   </si>
   <si>
     <t>5 way Intersection</t>
+  </si>
+  <si>
+    <t>NPC1.Lane</t>
+  </si>
+  <si>
+    <t>NPC1.Distance</t>
+  </si>
+  <si>
+    <t>NPC1.Acceleration</t>
+  </si>
+  <si>
+    <t>DUT.Lane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,6 +1050,12 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1780,29 +1798,29 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1955,30 +1973,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2244,29 +2262,29 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2475,29 +2493,29 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2639,29 +2657,29 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2766,30 +2784,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2852,20 +2870,10 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color theme="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2875,6 +2883,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="1"/>
@@ -2882,6 +2893,13 @@
         <top style="medium">
           <color theme="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -2898,15 +2916,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4135657D-4BFE-4926-8784-69046B31C8E0}" name="Table1" displayName="Table1" ref="A1:H25" totalsRowShown="0" headerRowBorderDxfId="93" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4135657D-4BFE-4926-8784-69046B31C8E0}" name="Table1" displayName="Table1" ref="A1:H25" totalsRowShown="0" headerRowBorderDxfId="94" tableBorderDxfId="93">
   <autoFilter ref="A1:H25" xr:uid="{94BC3B23-32FB-48E9-BC7C-486CB778E33F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BD1961A0-961D-4944-8E99-41CDDB2E1556}" name="ID"/>
     <tableColumn id="2" xr3:uid="{E5C1CC3B-7582-4795-84EE-0AD1F09ECC1A}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{295FC5F7-8FBB-487E-8EE3-76B36FA9AD2B}" name="lane (CAR2)"/>
-    <tableColumn id="4" xr3:uid="{5D2DAE2A-D866-4DDA-8399-2D8DC324A90D}" name="position (CAR2)"/>
-    <tableColumn id="5" xr3:uid="{442E7C19-642E-436B-8BB5-058519467302}" name="accel. (CAR2)" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{4CDC65E4-A515-433B-993B-4297666BABC6}" name="lane (DUT)"/>
+    <tableColumn id="3" xr3:uid="{295FC5F7-8FBB-487E-8EE3-76B36FA9AD2B}" name="NPC1.Lane"/>
+    <tableColumn id="4" xr3:uid="{5D2DAE2A-D866-4DDA-8399-2D8DC324A90D}" name="NPC1.Distance"/>
+    <tableColumn id="5" xr3:uid="{442E7C19-642E-436B-8BB5-058519467302}" name="NPC1.Acceleration" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{4CDC65E4-A515-433B-993B-4297666BABC6}" name="DUT.Lane"/>
     <tableColumn id="8" xr3:uid="{FEF7A40D-0533-42E1-A88C-0F545CF46B5C}" name="Reverse?"/>
     <tableColumn id="7" xr3:uid="{FC7F61F2-3EB4-4212-9EF1-98027AA0C78D}" name="Note"/>
   </tableColumns>
@@ -2915,7 +2933,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2EC1697-22B6-4BC2-BF72-2E8C06487613}" name="Table3" displayName="Table3" ref="A1:J17" totalsRowShown="0" headerRowBorderDxfId="90" tableBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2EC1697-22B6-4BC2-BF72-2E8C06487613}" name="Table3" displayName="Table3" ref="A1:J17" totalsRowShown="0" headerRowBorderDxfId="91" tableBorderDxfId="90">
   <autoFilter ref="A1:J17" xr:uid="{48F2E536-2070-49B3-A393-5160DDE6E9D6}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F777AE4A-7B05-4809-82E4-A9DD211871AD}" name="ID"/>
@@ -2951,7 +2969,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AFFA47CF-7050-1042-988A-97EF09D9E762}" name="Table4" displayName="Table4" ref="A1:E2" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AFFA47CF-7050-1042-988A-97EF09D9E762}" name="Table4" displayName="Table4" ref="A1:E2" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A1:E2" xr:uid="{2EFCBBDF-8509-FE40-8F82-33C908986358}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A191FB06-F4D0-A04A-A5F1-F666276311B8}" name="ID" dataDxfId="78"/>
@@ -2965,7 +2983,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D889457C-301E-3F42-99DB-FAA928FFC1FA}" name="Table9" displayName="Table9" ref="A1:G2" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" headerRowBorderDxfId="70" tableBorderDxfId="71" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D889457C-301E-3F42-99DB-FAA928FFC1FA}" name="Table9" displayName="Table9" ref="A1:G2" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="A1:G2" xr:uid="{E9C02C18-F408-D948-BCB8-7930E3A72EA4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{155CFBC4-7C33-624D-BD14-D2AB62D96E27}" name="ID" dataDxfId="68"/>
@@ -2981,7 +2999,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6E5FF8A2-777E-AB41-A03C-4A4A4D2EDD16}" name="Table8" displayName="Table8" ref="A1:K2" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" headerRowBorderDxfId="58" tableBorderDxfId="59" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6E5FF8A2-777E-AB41-A03C-4A4A4D2EDD16}" name="Table8" displayName="Table8" ref="A1:K2" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="A1:K2" xr:uid="{2E63B603-4ADB-C745-A900-2178BC350908}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{DDB41271-37B3-6F42-952F-4E550BA22BE0}" name="ID" dataDxfId="56"/>
@@ -3001,7 +3019,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{1D7F2870-98B0-3140-AD7B-8665DBFD6CA9}" name="Table10" displayName="Table10" ref="A1:M7" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{1D7F2870-98B0-3140-AD7B-8665DBFD6CA9}" name="Table10" displayName="Table10" ref="A1:M7" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="A1:M7" xr:uid="{E4961C86-6FB3-684E-963A-2B606F09B859}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C991A867-356F-3644-97F7-8D23087A243A}" name="ID" dataDxfId="40"/>
@@ -3023,7 +3041,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC930E04-6E07-0E49-9601-E28FC5D8735D}" name="Table5" displayName="Table5" ref="A1:H3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC930E04-6E07-0E49-9601-E28FC5D8735D}" name="Table5" displayName="Table5" ref="A1:H3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:H3" xr:uid="{36090C8C-DFDD-5348-8D2C-BC06ECAF7A2C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A889A05E-F87A-2A40-8D3D-C3A606B6FD6A}" name="ID" dataDxfId="22"/>
@@ -3040,7 +3058,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9DA943E7-D025-7542-A6D8-E8534EB5AB64}" name="Table11" displayName="Table11" ref="A1:J2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9DA943E7-D025-7542-A6D8-E8534EB5AB64}" name="Table11" displayName="Table11" ref="A1:J2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A1:J2" xr:uid="{4776D0A7-3399-7042-90C8-59372CCC15AD}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{68C67524-7E77-8145-968D-1A8246C010EE}" name="ID" dataDxfId="9"/>
@@ -3323,23 +3341,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="26" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3347,16 +3365,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>2</v>
+        <v>272</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>4</v>
+        <v>274</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="G1" s="84" t="s">
         <v>6</v>
@@ -3365,7 +3383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.25">
+    <row r="2" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>8</v>
       </c>
@@ -3387,7 +3405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>14</v>
       </c>
@@ -3407,7 +3425,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="110" t="s">
         <v>18</v>
       </c>
@@ -3427,7 +3445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.25">
+    <row r="5" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A5" s="103" t="s">
         <v>23</v>
       </c>
@@ -3445,7 +3463,7 @@
       <c r="G5" s="109"/>
       <c r="H5" s="65"/>
     </row>
-    <row r="6" spans="1:8" ht="29.25">
+    <row r="6" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A6" s="110" t="s">
         <v>26</v>
       </c>
@@ -3467,7 +3485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.25">
+    <row r="7" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A7" s="96" t="s">
         <v>29</v>
       </c>
@@ -3489,7 +3507,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.25">
+    <row r="8" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A8" s="88" t="s">
         <v>33</v>
       </c>
@@ -3511,7 +3529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
         <v>35</v>
       </c>
@@ -3531,7 +3549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>37</v>
       </c>
@@ -3548,7 +3566,7 @@
       </c>
       <c r="G10" s="87"/>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>41</v>
       </c>
@@ -3563,7 +3581,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:8" ht="29.25">
+    <row r="12" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A12" s="69" t="s">
         <v>45</v>
       </c>
@@ -3581,7 +3599,7 @@
       <c r="G12" s="66"/>
       <c r="H12" s="65"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>47</v>
       </c>
@@ -3596,7 +3614,7 @@
       </c>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
         <v>50</v>
       </c>
@@ -3614,7 +3632,7 @@
       <c r="G14" s="67"/>
       <c r="H14" s="65"/>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>54</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
         <v>56</v>
       </c>
@@ -3654,7 +3672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3669,7 +3687,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:8" ht="30">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
         <v>63</v>
       </c>
@@ -3691,7 +3709,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>66</v>
       </c>
@@ -3711,7 +3729,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>70</v>
       </c>
@@ -3733,7 +3751,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
         <v>74</v>
       </c>
@@ -3753,7 +3771,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
         <v>77</v>
       </c>
@@ -3773,7 +3791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -3793,7 +3811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="117" t="s">
         <v>84</v>
       </c>
@@ -3815,7 +3833,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="95" t="s">
         <v>88</v>
       </c>
@@ -3838,6 +3856,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3853,7 +3872,7 @@
       <selection activeCell="D17" sqref="D3:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -3866,7 +3885,7 @@
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
@@ -3901,7 +3920,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="132" t="s">
         <v>206</v>
       </c>
@@ -3952,7 +3971,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
@@ -3967,7 +3986,7 @@
     <col min="12" max="12" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21.95" customHeight="1">
+    <row r="1" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
@@ -4008,7 +4027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="63.95" customHeight="1">
+    <row r="2" spans="1:13" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="139" t="s">
         <v>223</v>
       </c>
@@ -4043,7 +4062,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="139" t="s">
         <v>223</v>
       </c>
@@ -4074,7 +4093,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60">
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="132" t="s">
         <v>231</v>
       </c>
@@ -4103,7 +4122,7 @@
       <c r="L4" s="133"/>
       <c r="M4" s="133"/>
     </row>
-    <row r="5" spans="1:13" ht="60">
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="143" t="s">
         <v>236</v>
       </c>
@@ -4136,7 +4155,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60">
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="143" t="s">
         <v>236</v>
       </c>
@@ -4167,7 +4186,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="146" customFormat="1" ht="60">
+    <row r="7" spans="1:13" s="146" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="139" t="s">
         <v>223</v>
       </c>
@@ -4196,7 +4215,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8" s="136"/>
       <c r="L8" s="136"/>
     </row>
@@ -4216,7 +4235,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
@@ -4225,7 +4244,7 @@
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="139" t="s">
         <v>244</v>
       </c>
@@ -4277,7 +4296,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="139" t="s">
         <v>250</v>
       </c>
@@ -4317,7 +4336,7 @@
       <selection activeCell="F13" sqref="F3:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
@@ -4328,7 +4347,7 @@
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
@@ -4360,7 +4379,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="66" customHeight="1">
+    <row r="2" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="132" t="s">
         <v>255</v>
       </c>
@@ -4408,7 +4427,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
@@ -4417,7 +4436,7 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>260</v>
       </c>
@@ -4425,7 +4444,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -4437,7 +4456,7 @@
       </c>
       <c r="E3" s="147"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>264</v>
       </c>
@@ -4448,7 +4467,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <v>4</v>
       </c>
@@ -4456,7 +4475,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
         <v>1</v>
       </c>
@@ -4464,7 +4483,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>264</v>
       </c>
@@ -4472,7 +4491,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="127" t="s">
         <v>268</v>
       </c>
@@ -4480,7 +4499,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>4</v>
       </c>
@@ -4488,7 +4507,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="126" t="s">
         <v>270</v>
       </c>
@@ -4509,7 +4528,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="56.85546875" customWidth="1"/>
@@ -4523,7 +4542,7 @@
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" thickBot="1">
+    <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
@@ -4555,7 +4574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4569,7 +4588,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -4583,7 +4602,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -4606,7 +4625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1">
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -4633,7 +4652,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4653,7 +4672,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -4667,7 +4686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -4687,7 +4706,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -4698,7 +4717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -4712,7 +4731,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>120</v>
       </c>
@@ -4738,7 +4757,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4749,7 +4768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>120</v>
       </c>
@@ -4775,7 +4794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>120</v>
       </c>
@@ -4801,7 +4820,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -4824,7 +4843,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>131</v>
       </c>
@@ -4844,7 +4863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -4880,7 +4899,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -4894,7 +4913,7 @@
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1">
+    <row r="1" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4932,7 +4951,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -4981,7 +5000,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" customWidth="1"/>
@@ -4992,7 +5011,7 @@
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5015,7 +5034,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -5048,7 +5067,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" customWidth="1"/>
@@ -5064,7 +5083,7 @@
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30.75" thickBot="1">
+    <row r="1" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5105,7 +5124,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -5141,7 +5160,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="51.7109375" style="15" customWidth="1"/>
@@ -5153,7 +5172,7 @@
     <col min="8" max="8" width="13.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" thickBot="1">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5179,7 +5198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>163</v>
       </c>
@@ -5199,7 +5218,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>168</v>
       </c>
@@ -5217,7 +5236,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>163</v>
       </c>
@@ -5237,7 +5256,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>168</v>
       </c>
@@ -5259,7 +5278,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>168</v>
       </c>
@@ -5277,7 +5296,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>163</v>
       </c>
@@ -5313,7 +5332,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -5325,7 +5344,7 @@
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45.75" thickBot="1">
+    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5360,7 +5379,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>181</v>
       </c>
@@ -5390,7 +5409,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
@@ -5402,7 +5421,7 @@
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="130" t="s">
         <v>0</v>
       </c>
@@ -5419,7 +5438,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" customHeight="1">
+    <row r="2" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="128" t="s">
         <v>186</v>
       </c>
@@ -5452,7 +5471,7 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
@@ -5461,7 +5480,7 @@
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
@@ -5484,7 +5503,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="62.1" customHeight="1">
+    <row r="2" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="132" t="s">
         <v>194</v>
       </c>
@@ -5742,13 +5761,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6352138-94E6-4006-A3A1-D79F276E2A77}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6352138-94E6-4006-A3A1-D79F276E2A77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4EE5297-04EB-4C34-AA22-C1F63E596189}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4EE5297-04EB-4C34-AA22-C1F63E596189}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41427505-FAFF-4BEE-B442-0F9294662C13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41427505-FAFF-4BEE-B442-0F9294662C13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="760962ba-41a6-4c22-8823-37e7800d07f7"/>
+    <ds:schemaRef ds:uri="908bafe6-243f-4184-9c59-db357c8fa058"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>